<commit_message>
update Test case New
</commit_message>
<xml_diff>
--- a/TEST CASE_SH_New_V0.xlsx
+++ b/TEST CASE_SH_New_V0.xlsx
@@ -5,25 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WOSS_NQCUONG\Smart_Home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WOSS_NQCUONG\Smart_Home\UPLOAD_GIT\-smart-home-DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Test case_Detail_Switch" sheetId="2" r:id="rId2"/>
     <sheet name="Test case_Detail_Gateway" sheetId="6" r:id="rId3"/>
     <sheet name="Test case_Detail_IR" sheetId="5" r:id="rId4"/>
-    <sheet name="Nhap" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="107">
   <si>
     <t>TC-01</t>
   </si>
@@ -80,21 +79,6 @@
   </si>
   <si>
     <t>TC-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRIAC: </t>
-  </si>
-  <si>
-    <t>Dẫn điện 2 chiều</t>
-  </si>
-  <si>
-    <t>Độ lớn dòng thông mạch k phụ thuộc độ lớn dòng điều khiển (khác với Transistor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khi đã mở thì vẫn giữ nguyên trạng thái cho tới khi áp đặt lên nó = 0 hoặc đảo chiều (không phải áp điều khiển) </t>
-  </si>
-  <si>
-    <t>Dẫn khi và chỉ khi có dòng điện/điện áp dương/âm đặt vào chân điều khiển</t>
   </si>
   <si>
     <t>Kiểm tra bật tắt bằng công tắc cơ</t>
@@ -576,16 +560,6 @@
       </rPr>
       <t xml:space="preserve"> tải.</t>
     </r>
-  </si>
-  <si>
-    <t>Điều khiển 1 máy lạnh bằng IR
-Các lệnh điều khiển:
-- Bật/Tắt
-- Nhiệt độ
-- Tốc độ gió
-- Swing
-- Hẹn giờ bật/tắt
-…</t>
   </si>
   <si>
     <r>
@@ -851,10 +825,6 @@
     <t>3 Bóng đèn sẽ sáng tắt theo thứ tự nhưng ách nhau khoảng thời gian rất ngắn (gần như cùng lúc)</t>
   </si>
   <si>
-    <t xml:space="preserve">1. 
-2.                                                                                                                                                                                                                                                                                                    </t>
-  </si>
-  <si>
     <t>Tương tác giữa cloud và Node thông qua Gateway
 Nhận yêu cầu từ cloud (Apps/người dùng)</t>
   </si>
@@ -904,17 +874,89 @@
 3. Từ máy tính A, truyền các lệnh cho gateway
 3. Theo dõi tín hiệu nhận được ở máy tính B và A</t>
   </si>
+  <si>
+    <t xml:space="preserve">Điều khiển 1 máy lạnh bằng IR
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Cấp nguồn mạch IR. 
+2. Kết nối mạch IR và điện thoại/mát tính bằng apps (nếu chưa có apps, có thể dùng tạm các apps nguồn mở). Sau đó thực hiện điều khiển máy lạnh
+Các lệnh điều khiển như:
+- Bật/Tắt
+- Nhiệt độ
+- Tốc độ gió
+- Swing
+- Hẹn giờ bật/tắt
+…                                                                                                                                                                                                                                                                                                   </t>
+  </si>
+  <si>
+    <t>5VDC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Có thể dùng nguồn 5VDC cấp cho mạch IR để test thay vì 220VAC. 
+Lưu ý:
+- Nếu cấp nguồn 5VDC thì cấp vào 2 chân đầu ra của mạch nguồn (Vcc &amp; GND)
+- Nếu cấp nguồn 220VAC-50Hz thì cấp vào 2 chân đầu vào mạch nguồn (L &amp; N). Chú ý đến </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AN TOÀN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>khi sử dụng điện dân dụng.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Giữ nguyên cách mắc như trên (TC-01), vừa điều khiển
+2. Đặt Node IR ra xa dần và điều khiển máy lạnh. Từ đó tìm được khoảng cách xa nhất ở mỗi trường hợp (có và không có housing)</t>
+  </si>
+  <si>
+    <t>1. Khoảng cách mà IR node điều khiển được trong cả 2 trường hợp phải &gt;10m
+2. Máy lạnh đáp ứng tức thì các lệnh điều khiển. Các lệnh truyền đi từ IR node không bị miss.</t>
+  </si>
+  <si>
+    <t>Có thể dùng nguồn 5VDC cấp cho mạch IR để test thay vì 220VAC. 
+Lưu ý:
+- Nếu cấp nguồn 5VDC thì cấp vào 2 chân đầu ra của mạch nguồn (Vcc &amp; GND)
+- Nếu cấp nguồn 220VAC-50Hz thì cấp vào 2 chân đầu vào mạch nguồn (L &amp; N). Chú ý đến AN TOÀN khi sử dụng điện dân dụng.</t>
+  </si>
+  <si>
+    <t>1.Máy lạnh đáp ứng tức thì các lệnh điều khiển. Các lệnh truyền đi từ IR node không bị miss.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1143,7 +1185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1776,87 +1818,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1865,353 +1917,371 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2542,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -2555,309 +2625,302 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="26.25">
       <c r="A2" s="6"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="71" t="s">
-        <v>51</v>
+      <c r="C2" s="27"/>
+      <c r="D2" s="49" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="39"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="53" t="s">
-        <v>52</v>
+      <c r="A4" s="45" t="s">
+        <v>47</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="72"/>
-      <c r="F4" s="30"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="50"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="B6" s="103" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="116"/>
+      <c r="M6" s="117"/>
     </row>
     <row r="7" spans="1:19" ht="30" customHeight="1">
-      <c r="A7" s="29"/>
-      <c r="B7" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="62">
+      <c r="A7" s="28"/>
+      <c r="B7" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="47">
         <v>1</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="90" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="52"/>
-      <c r="M7" s="60"/>
+      <c r="D7" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="114" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="106"/>
+      <c r="M7" s="107"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="29"/>
-      <c r="B8" s="65" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="111" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="44">
+        <v>2</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="49">
-        <v>2</v>
-      </c>
-      <c r="D8" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="60"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="107"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="47">
+      <c r="B9" s="112"/>
+      <c r="C9" s="42">
         <v>3</v>
       </c>
-      <c r="D9" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="52"/>
-      <c r="M9" s="60"/>
+      <c r="D9" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="106"/>
+      <c r="M9" s="107"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="47">
+      <c r="B10" s="112"/>
+      <c r="C10" s="42">
         <v>4</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="60"/>
+      <c r="D10" s="95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="106"/>
+      <c r="M10" s="107"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="27"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="47">
+      <c r="A11" s="26"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="42">
         <v>5</v>
       </c>
-      <c r="D11" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="97"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
+      <c r="D11" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="108" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="109"/>
+      <c r="M11" s="110"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68">
+      <c r="B12" s="113"/>
+      <c r="C12" s="48">
         <v>6</v>
       </c>
-      <c r="D12" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="99" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="100"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
+      <c r="D12" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="93"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
+      <c r="D13" s="37"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="6"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="F14" s="12"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="39"/>
-      <c r="F15" s="48"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
+      <c r="A15" s="34"/>
+      <c r="F15" s="43"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="6"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
     </row>
     <row r="17" spans="10:19">
-      <c r="J17" s="45"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
     </row>
     <row r="18" spans="10:19">
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
     </row>
     <row r="19" spans="10:19">
-      <c r="J19" s="43"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="K9:M9"/>
@@ -2866,6 +2929,13 @@
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2897,387 +2967,387 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A2" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
+      <c r="A2" s="133" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="135"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
+      <c r="A3" s="124" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="84" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="86"/>
+      <c r="A4" s="127" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="129"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A5" s="87" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
+      <c r="A5" s="130" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="132"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A7" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="35"/>
+      <c r="A7" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="142"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="142"/>
+      <c r="J7" s="143"/>
     </row>
     <row r="8" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="38" t="s">
+      <c r="I8" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="118" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="140" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60"/>
+    </row>
+    <row r="10" spans="1:10" ht="90.75" thickBot="1">
+      <c r="A10" s="137"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="122"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="63"/>
+      <c r="J10" s="64"/>
+    </row>
+    <row r="11" spans="1:10" ht="165">
+      <c r="A11" s="138" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="121" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="65"/>
+      <c r="J11" s="60"/>
+    </row>
+    <row r="12" spans="1:10" ht="165.75" thickBot="1">
+      <c r="A12" s="144"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="123"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="57"/>
+      <c r="J12" s="78"/>
+    </row>
+    <row r="13" spans="1:10" ht="120">
+      <c r="A13" s="138" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="121" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="54"/>
+      <c r="J13" s="60"/>
+    </row>
+    <row r="14" spans="1:10" ht="120.75" thickBot="1">
+      <c r="A14" s="137"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="122"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="69"/>
+      <c r="J14" s="64"/>
+    </row>
+    <row r="15" spans="1:10" ht="106.5" customHeight="1">
+      <c r="A15" s="136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="118" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="121" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="118" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="58"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="60"/>
+    </row>
+    <row r="16" spans="1:10" ht="106.5" customHeight="1" thickBot="1">
+      <c r="A16" s="137"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="122"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="119"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="64"/>
+    </row>
+    <row r="17" spans="1:10" ht="210.75" thickBot="1">
+      <c r="A17" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="76"/>
+    </row>
+    <row r="18" spans="1:10" ht="90.75" thickBot="1">
+      <c r="A18" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="76"/>
+    </row>
+    <row r="19" spans="1:10" ht="150.75" thickBot="1">
+      <c r="A19" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="94" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="103" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="94" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="107" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="109"/>
-    </row>
-    <row r="10" spans="1:10" ht="90.75" thickBot="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="112" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="112" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="114" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="115"/>
-      <c r="J10" s="116"/>
-    </row>
-    <row r="11" spans="1:10" ht="165">
-      <c r="A11" s="106" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="94" t="s">
+      <c r="D19" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="107" t="s">
+      <c r="F19" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="109"/>
-    </row>
-    <row r="12" spans="1:10" ht="165.75" thickBot="1">
-      <c r="A12" s="129"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="104"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="130" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="102"/>
-      <c r="J12" s="131"/>
-    </row>
-    <row r="13" spans="1:10" ht="120">
-      <c r="A13" s="106" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="122" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="107" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="109"/>
-    </row>
-    <row r="14" spans="1:10" ht="120.75" thickBot="1">
-      <c r="A14" s="110"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="118" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="141"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="119" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="118" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="120" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="121"/>
-      <c r="J14" s="116"/>
-    </row>
-    <row r="15" spans="1:10" ht="106.5" customHeight="1">
-      <c r="A15" s="132" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="73" t="s">
+      <c r="I19" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="76"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="60"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A21" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="93" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="122" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="73" t="s">
-        <v>100</v>
-      </c>
-      <c r="H15" s="107"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="109"/>
-    </row>
-    <row r="16" spans="1:10" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A16" s="110"/>
-      <c r="B16" s="111"/>
-      <c r="C16" s="118" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="141"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="119" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="113"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="116"/>
-    </row>
-    <row r="17" spans="1:10" ht="210.75" thickBot="1">
-      <c r="A17" s="133" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="124" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="125" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="124" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="125" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="125" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="126" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="127" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="128"/>
-    </row>
-    <row r="18" spans="1:10" ht="90.75" thickBot="1">
-      <c r="A18" s="133" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="124" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="125" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="124" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="125" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="125" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="126" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="127" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="128"/>
-    </row>
-    <row r="19" spans="1:10" ht="150.75" thickBot="1">
-      <c r="A19" s="133" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="124" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="125" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="124" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="125" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="125" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="126" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="127" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" s="128"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="134" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="109"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A21" s="137" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="139"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="138"/>
-      <c r="I21" s="140"/>
-      <c r="J21" s="116"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="64"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="5"/>
@@ -3365,12 +3435,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D15:D16"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
@@ -3380,15 +3444,21 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3398,8 +3468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3412,105 +3482,107 @@
     <col min="6" max="6" width="30.28515625" customWidth="1"/>
     <col min="7" max="7" width="41.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
+      <c r="A2" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A4" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="35"/>
+      <c r="A4" s="141" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="142"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="143"/>
     </row>
     <row r="5" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="38" t="s">
+      <c r="I5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="210">
-      <c r="A6" s="94" t="s">
+    <row r="6" spans="1:10" ht="340.5" customHeight="1">
+      <c r="A6" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="93" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>103</v>
+      <c r="B6" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="154" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="8" t="s">
         <v>13</v>
       </c>
@@ -3518,15 +3590,15 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="8" t="s">
         <v>13</v>
       </c>
@@ -3537,77 +3609,77 @@
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="22"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="19"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="21"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="22"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="26"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="16"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="26"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="26"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="16"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="26"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="16"/>
-      <c r="B15" s="23"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
@@ -3714,8 +3786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3729,213 +3801,221 @@
     <col min="7" max="7" width="41.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A2" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="35"/>
+      <c r="A2" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="143"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" customHeight="1">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="105" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="93" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="73" t="s">
+      <c r="B4" s="148" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="145" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="147" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="149" t="s">
+      <c r="F4" s="149" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="149" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="108"/>
-      <c r="J4" s="109"/>
-    </row>
-    <row r="5" spans="1:10" ht="75" customHeight="1" thickBot="1">
-      <c r="A5" s="110"/>
-      <c r="B5" s="143"/>
-      <c r="C5" s="143"/>
-      <c r="D5" s="118" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="150" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="152" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="119.25" customHeight="1" thickBot="1">
+      <c r="A5" s="137"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="155" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="119"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="144"/>
-      <c r="J5" s="145"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="150"/>
     </row>
     <row r="6" spans="1:10" ht="75" customHeight="1">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="135" t="s">
+      <c r="B6" s="118" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="118" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="149" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="149" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="146"/>
-      <c r="J6" s="147"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="150"/>
     </row>
     <row r="7" spans="1:10" ht="75" customHeight="1" thickBot="1">
-      <c r="A7" s="110"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="118" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="113"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="118" t="s">
+      <c r="A7" s="137"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="119"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="140"/>
-      <c r="J7" s="116"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="151"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="13"/>
-      <c r="B8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="22"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="14"/>
-      <c r="B9" s="21"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="21"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="21"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="16"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="26"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="16"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="26"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="26"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="16"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
@@ -3946,7 +4026,7 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4042,7 +4122,11 @@
       <c r="J23" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
@@ -4053,64 +4137,8 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2" spans="2:17">
-      <c r="B2" s="12"/>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4" s="12"/>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="12"/>
-    </row>
-    <row r="6" spans="2:17">
-      <c r="B6" s="12"/>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="B7" s="15"/>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="Q15" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="Q16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="17:17">
-      <c r="Q17" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="17:17">
-      <c r="Q18" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="17:17">
-      <c r="Q19" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update day 4, time 2
</commit_message>
<xml_diff>
--- a/TEST CASE_SH_New_V0.xlsx
+++ b/TEST CASE_SH_New_V0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="804"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="804" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="152">
   <si>
     <t>TC-01</t>
   </si>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>Bật tắt relay liên tục</t>
-  </si>
-  <si>
-    <t>TC-09</t>
   </si>
   <si>
     <r>
@@ -1412,17 +1409,106 @@
   <si>
     <t>Test hoạt động của Dimmer</t>
   </si>
+  <si>
+    <t>Tên 
+Test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test khả năng lọc nhiễu dưới tác động của:
+- Máy khoan
+- Máy hàn điện </t>
+  </si>
+  <si>
+    <t>Test ảnh hưởng bởi các yếu tố bên ngoài</t>
+  </si>
+  <si>
+    <t>Các bóng đèn vẫn tắt mở với chu kỳ 1s 1 lần</t>
+  </si>
+  <si>
+    <t>Test khả năng chống sét của thiết bị???</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Các bước chuẩn bị và cách mắc tương tự như phần kiểm tra bật tắt bằng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MCU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> của </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TC-02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Dùng Terminal gửi tín hiệu bật tắt đèn 1s 1 lần tới Switch
+3. Chạy máy khoan tường công suất lớn (chỉ nhấn cho mũi khoan xoay, không khoan vào tường. Chú ý đến an toàn) ngay bên cạnh Switch. Theo dõi xem đèn có sáng tắt như lúc chưa có máy khoan không.
+4. Tương tự với máy hàn điện</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Giữ nguyên cách mắc và kết nối như ở các phần trên
+2. Chạy máy khoan tường công suất lớn (chỉ nhấn cho mũi khoan xoay, không khoan vào tường. Chú ý đến an toàn) ngay bên cạnh máy lạnh. 
+3. Điều khiển máy lạnh bằng IR. Theo dõi xem máy lạnh có hoạt động như mong muốn không
+4. Tương tự với máy hàn điện</t>
+  </si>
+  <si>
+    <t>Máy lạnh hoạt động như theo lệnh của IR. Không bị ảnh hưởng bởi nhiễu</t>
+  </si>
+  <si>
+    <t>Test ảnh hưởng nhiễu bởi các yếu tố bên ngoài</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2362,666 +2448,693 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3352,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:J9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3365,299 +3478,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="26.25">
       <c r="A2" s="6"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="44" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="49" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="33"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="40" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="49"/>
-      <c r="F4" s="29"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="45"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="135" t="s">
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="136"/>
-      <c r="M6" s="137"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="132"/>
     </row>
     <row r="7" spans="1:19" ht="30" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="45" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="42">
         <v>1</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="134" t="s">
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="129"/>
-      <c r="M7" s="130"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="125"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="28"/>
-      <c r="B8" s="131" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="39">
         <v>2</v>
       </c>
-      <c r="D8" s="145" t="s">
+      <c r="D8" s="140" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="146"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="128" t="s">
+      <c r="E8" s="141"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="129"/>
-      <c r="M8" s="130"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="125"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6"/>
-      <c r="B9" s="132"/>
-      <c r="C9" s="41">
+      <c r="B9" s="127"/>
+      <c r="C9" s="37">
         <v>3</v>
       </c>
-      <c r="D9" s="141" t="s">
+      <c r="D9" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="128" t="s">
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="129"/>
-      <c r="M9" s="130"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="125"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6"/>
-      <c r="B10" s="132"/>
-      <c r="C10" s="41">
+      <c r="B10" s="127"/>
+      <c r="C10" s="37">
         <v>4</v>
       </c>
-      <c r="D10" s="147" t="s">
+      <c r="D10" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="142"/>
-      <c r="J10" s="142"/>
-      <c r="K10" s="128" t="s">
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="129"/>
-      <c r="M10" s="130"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="125"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="26"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="41">
+      <c r="A11" s="22"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="37">
         <v>5</v>
       </c>
-      <c r="D11" s="148" t="s">
+      <c r="D11" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="142"/>
-      <c r="F11" s="142"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="142"/>
-      <c r="I11" s="142"/>
-      <c r="J11" s="142"/>
-      <c r="K11" s="128" t="s">
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="129"/>
-      <c r="M11" s="130"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="125"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="47">
+      <c r="B12" s="128"/>
+      <c r="C12" s="43">
         <v>6</v>
       </c>
-      <c r="D12" s="149" t="s">
+      <c r="D12" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="150"/>
-      <c r="F12" s="150"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="150"/>
-      <c r="I12" s="150"/>
-      <c r="J12" s="150"/>
-      <c r="K12" s="138" t="s">
-        <v>122</v>
-      </c>
-      <c r="L12" s="139"/>
-      <c r="M12" s="140"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="133" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="134"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6"/>
-      <c r="B13" s="35"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
+      <c r="D13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="6"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
       <c r="F14" s="12"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="33"/>
-      <c r="F15" s="42"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
+      <c r="A15" s="29"/>
+      <c r="F15" s="38"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="6"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
     </row>
     <row r="17" spans="10:19">
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
     </row>
     <row r="18" spans="10:19">
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="40"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
     </row>
     <row r="19" spans="10:19">
-      <c r="J19" s="37"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3687,15 +3800,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" customWidth="1"/>
@@ -3707,409 +3820,419 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="182" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
-      <c r="F2" s="161" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="162"/>
+      <c r="A2" s="169" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
+      <c r="F2" s="146" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="147"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="160" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="175"/>
-      <c r="F3" s="163" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="164"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
+      <c r="F3" s="148" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="149"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="178"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="166"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="151"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="120"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="166"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="112"/>
+      <c r="F5" s="150"/>
+      <c r="G5" s="151"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A6" s="179" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="180"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="F6" s="167"/>
-      <c r="G6" s="168"/>
+      <c r="A6" s="166" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="167"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="168"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="153"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A8" s="154" t="s">
+      <c r="A8" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="155"/>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="155"/>
-      <c r="J8" s="156"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="178"/>
+      <c r="F8" s="178"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="178"/>
+      <c r="J8" s="179"/>
     </row>
     <row r="9" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="90">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="169" t="s">
+      <c r="D10" s="156" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="172" t="s">
+      <c r="E10" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="55"/>
-      <c r="J10" s="56"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:10" ht="90.75" thickBot="1">
-      <c r="A11" s="160"/>
-      <c r="B11" s="157"/>
-      <c r="C11" s="57" t="s">
+      <c r="A11" s="173"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="170"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="57" t="s">
+      <c r="D11" s="157"/>
+      <c r="E11" s="155"/>
+      <c r="F11" s="223" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:10" ht="165">
-      <c r="A12" s="158" t="s">
+      <c r="A12" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="151" t="s">
+      <c r="B12" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="169" t="s">
+      <c r="D12" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="151" t="s">
+      <c r="E12" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="220" t="s">
+      <c r="F12" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="54" t="s">
+      <c r="H12" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="61"/>
-      <c r="J12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:10" ht="165.75" thickBot="1">
-      <c r="A13" s="159"/>
-      <c r="B13" s="153"/>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="180"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="171"/>
-      <c r="E13" s="153"/>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="158"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="53"/>
-      <c r="J13" s="74"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="70"/>
     </row>
     <row r="14" spans="1:10" ht="120">
-      <c r="A14" s="158" t="s">
+      <c r="A14" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="169" t="s">
+      <c r="D14" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="151" t="s">
+      <c r="E14" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="54" t="s">
+      <c r="H14" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="50"/>
-      <c r="J14" s="56"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:10" ht="120.75" thickBot="1">
-      <c r="A15" s="160"/>
-      <c r="B15" s="157"/>
-      <c r="C15" s="62" t="s">
+      <c r="A15" s="173"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="170"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="63" t="s">
+      <c r="D15" s="157"/>
+      <c r="E15" s="155"/>
+      <c r="F15" s="225" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="61"/>
+      <c r="J15" s="56"/>
+    </row>
+    <row r="16" spans="1:10" ht="106.5" customHeight="1">
+      <c r="A16" s="172" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="154" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="156" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="154" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="64" t="s">
+      <c r="G16" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="50"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="52"/>
+    </row>
+    <row r="17" spans="1:10" ht="106.5" customHeight="1" thickBot="1">
+      <c r="A17" s="173"/>
+      <c r="B17" s="155"/>
+      <c r="C17" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="157"/>
+      <c r="E17" s="155"/>
+      <c r="F17" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="175"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="56"/>
+    </row>
+    <row r="18" spans="1:10" ht="210.75" thickBot="1">
+      <c r="A18" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="65"/>
-      <c r="J15" s="60"/>
-    </row>
-    <row r="16" spans="1:10" ht="106.5" customHeight="1">
-      <c r="A16" s="185" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="151" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="169" t="s">
+      <c r="I18" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="68"/>
+    </row>
+    <row r="19" spans="1:10" ht="90.75" thickBot="1">
+      <c r="A19" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="151" t="s">
+      <c r="E19" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="151" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="56"/>
-    </row>
-    <row r="17" spans="1:10" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A17" s="160"/>
-      <c r="B17" s="157"/>
-      <c r="C17" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="170"/>
-      <c r="E17" s="157"/>
-      <c r="F17" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="152"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="60"/>
-    </row>
-    <row r="18" spans="1:10" ht="210.75" thickBot="1">
-      <c r="A18" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="83" t="s">
+      <c r="F19" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="68"/>
+    </row>
+    <row r="20" spans="1:10" ht="150.75" thickBot="1">
+      <c r="A20" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="E20" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="70" t="s">
+      <c r="F20" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="72"/>
-    </row>
-    <row r="19" spans="1:10" ht="90.75" thickBot="1">
-      <c r="A19" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="83" t="s">
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
+    </row>
+    <row r="21" spans="1:10" ht="195">
+      <c r="A21" s="172" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="220" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="218" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="228" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="68" t="s">
+      <c r="E21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" s="72"/>
-    </row>
-    <row r="20" spans="1:10" ht="150.75" thickBot="1">
-      <c r="A20" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="83" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="72"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="56"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A22" s="79" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="60"/>
+      <c r="F21" s="218" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="218" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="52"/>
+    </row>
+    <row r="22" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A22" s="219"/>
+      <c r="B22" s="221"/>
+      <c r="C22" s="229" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="226"/>
+      <c r="E22" s="227"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="5"/>
@@ -4196,7 +4319,17 @@
       <c r="J30" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G6"/>
     <mergeCell ref="E16:E17"/>
@@ -4213,16 +4346,8 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4232,7 +4357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -4252,289 +4377,289 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="184" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="186"/>
+      <c r="F2" s="190" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="191"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="187" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="189"/>
+      <c r="F3" s="192" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="188"/>
-      <c r="F2" s="192" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="193"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="189" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="F3" s="194" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="195"/>
+      <c r="G3" s="193"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="E4" s="93"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="93"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A6" s="154" t="s">
+      <c r="A6" s="177" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="156"/>
+      <c r="B6" s="178"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="178"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="179"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="235.5" customHeight="1">
-      <c r="A8" s="101" t="s">
+      <c r="A8" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="196" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="90" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="196" t="s">
+      <c r="B8" s="194" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="194" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="216" t="s">
+      <c r="E8" s="197" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="90" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="96" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="54" t="s">
+      <c r="F8" s="82" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="199" t="s">
-        <v>142</v>
+      <c r="I8" s="51"/>
+      <c r="J8" s="181" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="93.75" customHeight="1">
-      <c r="A9" s="102" t="s">
+      <c r="A9" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="197"/>
-      <c r="C9" s="92" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="91" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" s="97" t="s">
-        <v>103</v>
+      <c r="B9" s="195"/>
+      <c r="C9" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="89" t="s">
+        <v>102</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="200"/>
+      <c r="J9" s="182"/>
     </row>
     <row r="10" spans="1:10" ht="120.75" customHeight="1">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="197"/>
-      <c r="C10" s="91" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="91" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="91" t="s">
-        <v>102</v>
+      <c r="B10" s="195"/>
+      <c r="C10" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="83" t="s">
+        <v>101</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="200"/>
+      <c r="J10" s="182"/>
     </row>
     <row r="11" spans="1:10" ht="119.25" customHeight="1">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="198"/>
-      <c r="C11" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="198"/>
-      <c r="E11" s="198"/>
-      <c r="F11" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="91" t="s">
-        <v>109</v>
+      <c r="B11" s="196"/>
+      <c r="C11" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="196"/>
+      <c r="E11" s="196"/>
+      <c r="F11" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="83" t="s">
+        <v>108</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="200"/>
+      <c r="J11" s="182"/>
     </row>
     <row r="12" spans="1:10" ht="186.75" customHeight="1" thickBot="1">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="182"/>
+    </row>
+    <row r="13" spans="1:10" ht="160.5" customHeight="1">
+      <c r="A13" s="100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="88" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="95" t="s">
+      <c r="D13" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="92" t="s">
+      <c r="E13" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="92" t="s">
+      <c r="F13" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="63"/>
+      <c r="J13" s="182"/>
+    </row>
+    <row r="14" spans="1:10" ht="138" customHeight="1" thickBot="1">
+      <c r="A14" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="97" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="97" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="97" t="s">
         <v>124</v>
       </c>
-      <c r="H12" s="111" t="s">
+      <c r="H14" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="200"/>
-    </row>
-    <row r="13" spans="1:10" ht="160.5" customHeight="1">
-      <c r="A13" s="108" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="96" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="96" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="107" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="96" t="s">
-        <v>126</v>
-      </c>
-      <c r="H13" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="67"/>
-      <c r="J13" s="200"/>
-    </row>
-    <row r="14" spans="1:10" ht="138" customHeight="1" thickBot="1">
-      <c r="A14" s="109" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="105" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="112" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="113" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="105" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="105" t="s">
-        <v>125</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="201"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="183"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="106"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="17"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="15"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="25"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="15"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
@@ -4547,7 +4672,7 @@
     <row r="19" spans="1:10">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="114"/>
+      <c r="C19" s="106"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -4649,8 +4774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4669,239 +4794,259 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="184" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="186"/>
+      <c r="F2" s="190" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="191"/>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
+      <c r="A3" s="187" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="189"/>
+      <c r="F3" s="192" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="188"/>
-      <c r="F2" s="192" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="193"/>
-    </row>
-    <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A3" s="189" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="F3" s="194" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="195"/>
+      <c r="G3" s="193"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A5" s="154" t="s">
+      <c r="A5" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="155"/>
-      <c r="J5" s="156"/>
+      <c r="B5" s="178"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="179"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" customHeight="1">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="205" t="s">
+      <c r="B7" s="201" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="203" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="200" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="198" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="207" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="50" t="s">
+      <c r="G7" s="198" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="51"/>
+      <c r="J7" s="107"/>
+    </row>
+    <row r="8" spans="1:10" ht="119.25" customHeight="1" thickBot="1">
+      <c r="A8" s="173"/>
+      <c r="B8" s="202"/>
+      <c r="C8" s="202"/>
+      <c r="D8" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="175"/>
+      <c r="F8" s="157"/>
+      <c r="G8" s="199"/>
+      <c r="H8" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="76"/>
+      <c r="J8" s="109"/>
+    </row>
+    <row r="9" spans="1:10" ht="68.25" customHeight="1">
+      <c r="A9" s="172" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="154" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="154" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="204" t="s">
+      <c r="E9" s="220" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="202" t="s">
+      <c r="G9" s="198" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="109"/>
+    </row>
+    <row r="10" spans="1:10" ht="69" customHeight="1" thickBot="1">
+      <c r="A10" s="173"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="222" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="175"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="222" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="74"/>
+      <c r="J10" s="108"/>
+    </row>
+    <row r="11" spans="1:10" ht="87" customHeight="1">
+      <c r="A11" s="232" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="220" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="230" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="220" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="202" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="86" t="s">
+      <c r="F11" s="230" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="230" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="218" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="115"/>
-    </row>
-    <row r="8" spans="1:10" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A8" s="160"/>
-      <c r="B8" s="206"/>
-      <c r="C8" s="206"/>
-      <c r="D8" s="89" t="s">
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:10" ht="86.25" customHeight="1" thickBot="1">
+      <c r="A12" s="233"/>
+      <c r="B12" s="221"/>
+      <c r="C12" s="234"/>
+      <c r="D12" s="222" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="152"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="203"/>
-      <c r="H8" s="87" t="s">
+      <c r="E12" s="221"/>
+      <c r="F12" s="234"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="222" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="117"/>
-    </row>
-    <row r="9" spans="1:10" ht="75" customHeight="1">
-      <c r="A9" s="185" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="151" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="151" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="204" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="202" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="202" t="s">
-        <v>96</v>
-      </c>
-      <c r="H9" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="117"/>
-    </row>
-    <row r="10" spans="1:10" ht="75" customHeight="1" thickBot="1">
-      <c r="A10" s="160"/>
-      <c r="B10" s="152"/>
-      <c r="C10" s="152"/>
-      <c r="D10" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="152"/>
-      <c r="F10" s="203"/>
-      <c r="G10" s="203"/>
-      <c r="H10" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="82"/>
-      <c r="J10" s="116"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="14"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="10"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="231"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="15"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="25"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="15"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
@@ -4912,7 +5057,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5008,7 +5153,18 @@
       <c r="J26" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="23">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A9:A10"/>
@@ -5021,11 +5177,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5036,8 +5187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5056,162 +5207,162 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="182" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
-      <c r="F2" s="192" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="193"/>
+      <c r="A2" s="169" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
+      <c r="F2" s="190" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="191"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="223" t="s">
+      <c r="A3" s="204" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="225"/>
-      <c r="F3" s="211" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="212"/>
+      <c r="B3" s="205"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="206"/>
+      <c r="F3" s="207" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="208"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="125"/>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="124"/>
-      <c r="B5" s="124"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="125"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="18.75">
-      <c r="A8" s="210" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="210"/>
-      <c r="C8" s="210"/>
-      <c r="D8" s="210"/>
-      <c r="E8" s="210"/>
-      <c r="F8" s="210"/>
-      <c r="G8" s="210"/>
-      <c r="H8" s="210"/>
-      <c r="I8" s="210"/>
-      <c r="J8" s="210"/>
+      <c r="A8" s="209" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="209"/>
+      <c r="C8" s="209"/>
+      <c r="D8" s="209"/>
+      <c r="E8" s="209"/>
+      <c r="F8" s="209"/>
+      <c r="G8" s="209"/>
+      <c r="H8" s="209"/>
+      <c r="I8" s="209"/>
+      <c r="J8" s="209"/>
     </row>
     <row r="9" spans="1:10" ht="30">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="121" t="s">
+      <c r="D9" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="121" t="s">
+      <c r="E9" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="121" t="s">
+      <c r="F9" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="121" t="s">
+      <c r="G9" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="121" t="s">
+      <c r="H9" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="122" t="s">
+      <c r="I9" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="122" t="s">
+      <c r="J9" s="114" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105">
-      <c r="A10" s="123" t="s">
+      <c r="A10" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="214" t="s">
+      <c r="B10" s="118" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="118" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="210" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="212" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="214" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="215" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="213" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="214" t="s">
+      <c r="G10" s="216" t="s">
         <v>138</v>
-      </c>
-      <c r="G10" s="221" t="s">
-        <v>139</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="218" t="s">
-        <v>141</v>
+      <c r="J10" s="214" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="111" customHeight="1">
-      <c r="A11" s="217" t="s">
+      <c r="A11" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="214" t="s">
+      <c r="B11" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="214" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="209"/>
-      <c r="E11" s="208"/>
-      <c r="F11" s="214" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="222"/>
+      <c r="D11" s="211"/>
+      <c r="E11" s="213"/>
+      <c r="F11" s="118" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="217"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="219"/>
+      <c r="J11" s="215"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="217" t="s">
+      <c r="A12" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
@@ -5222,7 +5373,7 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="217" t="s">
+      <c r="A13" s="119" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3"/>
@@ -5321,15 +5472,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="G10:G11"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A8:J8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
up HDSD lap dat Node
</commit_message>
<xml_diff>
--- a/TEST CASE_SH_New_V0.xlsx
+++ b/TEST CASE_SH_New_V0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="804" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1496,12 +1496,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2448,360 +2455,390 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2810,73 +2847,103 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="32" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2894,248 +2961,185 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3465,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:J7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3517,22 +3521,22 @@
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="130" t="s">
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="140" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="131"/>
-      <c r="M6" s="132"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="142"/>
     </row>
     <row r="7" spans="1:19" ht="30" customHeight="1">
       <c r="A7" s="24"/>
@@ -3542,106 +3546,106 @@
       <c r="C7" s="42">
         <v>1</v>
       </c>
-      <c r="D7" s="138" t="s">
+      <c r="D7" s="231" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="139"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="129" t="s">
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="124"/>
-      <c r="M7" s="125"/>
+      <c r="L7" s="134"/>
+      <c r="M7" s="135"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="24"/>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="136" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="39">
         <v>2</v>
       </c>
-      <c r="D8" s="140" t="s">
+      <c r="D8" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="141"/>
-      <c r="H8" s="141"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="123" t="s">
+      <c r="E8" s="148"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="148"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="148"/>
+      <c r="K8" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="124"/>
-      <c r="M8" s="125"/>
+      <c r="L8" s="134"/>
+      <c r="M8" s="135"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="37">
         <v>3</v>
       </c>
-      <c r="D9" s="136" t="s">
+      <c r="D9" s="233" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="137"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="123" t="s">
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="124"/>
-      <c r="M9" s="125"/>
+      <c r="L9" s="134"/>
+      <c r="M9" s="135"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6"/>
-      <c r="B10" s="127"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="37">
         <v>4</v>
       </c>
-      <c r="D10" s="142" t="s">
+      <c r="D10" s="233" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="137"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="123" t="s">
+      <c r="E10" s="146"/>
+      <c r="F10" s="146"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="124"/>
-      <c r="M10" s="125"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="135"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="22"/>
-      <c r="B11" s="127"/>
+      <c r="B11" s="137"/>
       <c r="C11" s="37">
         <v>5</v>
       </c>
-      <c r="D11" s="143" t="s">
+      <c r="D11" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="123" t="s">
+      <c r="E11" s="146"/>
+      <c r="F11" s="146"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="146"/>
+      <c r="J11" s="146"/>
+      <c r="K11" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="124"/>
-      <c r="M11" s="125"/>
+      <c r="L11" s="134"/>
+      <c r="M11" s="135"/>
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
@@ -3651,24 +3655,24 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="128"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="43">
         <v>6</v>
       </c>
-      <c r="D12" s="144" t="s">
+      <c r="D12" s="150" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="145"/>
-      <c r="K12" s="133" t="s">
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="151"/>
+      <c r="K12" s="143" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="134"/>
-      <c r="M12" s="135"/>
+      <c r="L12" s="144"/>
+      <c r="M12" s="145"/>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
@@ -3820,38 +3824,38 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="187" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
-      <c r="F2" s="146" t="s">
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="189"/>
+      <c r="F2" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="147"/>
+      <c r="G2" s="167"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="162"/>
-      <c r="F3" s="148" t="s">
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="180"/>
+      <c r="F3" s="168" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="149"/>
+      <c r="G3" s="169"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="163" t="s">
+      <c r="A4" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="164"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="151"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="183"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="171"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="110" t="s">
@@ -3860,33 +3864,33 @@
       <c r="B5" s="111"/>
       <c r="C5" s="111"/>
       <c r="D5" s="112"/>
-      <c r="F5" s="150"/>
-      <c r="G5" s="151"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="184" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="167"/>
-      <c r="C6" s="167"/>
-      <c r="D6" s="168"/>
-      <c r="F6" s="152"/>
-      <c r="G6" s="153"/>
+      <c r="B6" s="185"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="186"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="178"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="178"/>
-      <c r="E8" s="178"/>
-      <c r="F8" s="178"/>
-      <c r="G8" s="178"/>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="160"/>
+      <c r="D8" s="160"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="161"/>
     </row>
     <row r="9" spans="1:10" ht="30.75" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -3921,19 +3925,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="90">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="156" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="156" t="s">
+      <c r="D10" s="174" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="159" t="s">
+      <c r="E10" s="177" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -3949,14 +3953,14 @@
       <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:10" ht="90.75" thickBot="1">
-      <c r="A11" s="173"/>
-      <c r="B11" s="155"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="157"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="223" t="s">
+      <c r="D11" s="175"/>
+      <c r="E11" s="162"/>
+      <c r="F11" s="123" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="53" t="s">
@@ -3969,19 +3973,19 @@
       <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:10" ht="165">
-      <c r="A12" s="174" t="s">
+      <c r="A12" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="154" t="s">
+      <c r="B12" s="156" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="156" t="s">
+      <c r="D12" s="174" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="154" t="s">
+      <c r="E12" s="156" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="120" t="s">
@@ -3997,14 +4001,14 @@
       <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:10" ht="165.75" thickBot="1">
-      <c r="A13" s="180"/>
-      <c r="B13" s="176"/>
+      <c r="A13" s="164"/>
+      <c r="B13" s="158"/>
       <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="158"/>
-      <c r="E13" s="176"/>
-      <c r="F13" s="224" t="s">
+      <c r="D13" s="176"/>
+      <c r="E13" s="158"/>
+      <c r="F13" s="124" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="20" t="s">
@@ -4017,19 +4021,19 @@
       <c r="J13" s="70"/>
     </row>
     <row r="14" spans="1:10" ht="120">
-      <c r="A14" s="174" t="s">
+      <c r="A14" s="163" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="156" t="s">
         <v>83</v>
       </c>
       <c r="C14" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="156" t="s">
+      <c r="D14" s="174" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="154" t="s">
+      <c r="E14" s="156" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="62" t="s">
@@ -4045,14 +4049,14 @@
       <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:10" ht="120.75" thickBot="1">
-      <c r="A15" s="173"/>
-      <c r="B15" s="155"/>
+      <c r="A15" s="165"/>
+      <c r="B15" s="162"/>
       <c r="C15" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="157"/>
-      <c r="E15" s="155"/>
-      <c r="F15" s="225" t="s">
+      <c r="D15" s="175"/>
+      <c r="E15" s="162"/>
+      <c r="F15" s="125" t="s">
         <v>84</v>
       </c>
       <c r="G15" s="58" t="s">
@@ -4065,25 +4069,25 @@
       <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" ht="106.5" customHeight="1">
-      <c r="A16" s="172" t="s">
+      <c r="A16" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="156" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="156" t="s">
+      <c r="D16" s="174" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="156" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="154" t="s">
+      <c r="G16" s="156" t="s">
         <v>90</v>
       </c>
       <c r="H16" s="50"/>
@@ -4091,17 +4095,17 @@
       <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:10" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A17" s="173"/>
-      <c r="B17" s="155"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="162"/>
       <c r="C17" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="157"/>
-      <c r="E17" s="155"/>
+      <c r="D17" s="175"/>
+      <c r="E17" s="162"/>
       <c r="F17" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="175"/>
+      <c r="G17" s="157"/>
       <c r="H17" s="60"/>
       <c r="I17" s="61"/>
       <c r="J17" s="56"/>
@@ -4195,25 +4199,25 @@
       <c r="J20" s="68"/>
     </row>
     <row r="21" spans="1:10" ht="195">
-      <c r="A21" s="172" t="s">
+      <c r="A21" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="220" t="s">
+      <c r="B21" s="154" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="218" t="s">
+      <c r="C21" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="228" t="s">
+      <c r="D21" s="128" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="218" t="s">
+      <c r="F21" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="G21" s="218" t="s">
+      <c r="G21" s="121" t="s">
         <v>146</v>
       </c>
       <c r="H21" s="50"/>
@@ -4221,13 +4225,13 @@
       <c r="J21" s="52"/>
     </row>
     <row r="22" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A22" s="219"/>
-      <c r="B22" s="221"/>
-      <c r="C22" s="229" t="s">
+      <c r="A22" s="153"/>
+      <c r="B22" s="155"/>
+      <c r="C22" s="129" t="s">
         <v>147</v>
       </c>
-      <c r="D22" s="226"/>
-      <c r="E22" s="227"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
       <c r="F22" s="73"/>
       <c r="G22" s="73"/>
       <c r="H22" s="73"/>
@@ -4320,16 +4324,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G6"/>
     <mergeCell ref="E16:E17"/>
@@ -4346,8 +4340,18 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4377,28 +4381,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="193" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="186"/>
-      <c r="F2" s="190" t="s">
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="195"/>
+      <c r="F2" s="199" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="191"/>
+      <c r="G2" s="200"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="188"/>
-      <c r="D3" s="189"/>
-      <c r="F3" s="192" t="s">
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="F3" s="201" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="193"/>
+      <c r="G3" s="202"/>
     </row>
     <row r="4" spans="1:10">
       <c r="E4" s="85"/>
@@ -4408,18 +4412,18 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="178"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="178"/>
-      <c r="G6" s="178"/>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="179"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="161"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" thickBot="1">
       <c r="A7" s="26" t="s">
@@ -4457,16 +4461,16 @@
       <c r="A8" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="194" t="s">
+      <c r="B8" s="203" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="194" t="s">
+      <c r="D8" s="203" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="197" t="s">
+      <c r="E8" s="206" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="82" t="s">
@@ -4479,7 +4483,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="51"/>
-      <c r="J8" s="181" t="s">
+      <c r="J8" s="190" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4487,12 +4491,12 @@
       <c r="A9" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="195"/>
+      <c r="B9" s="204"/>
       <c r="C9" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="195"/>
-      <c r="E9" s="195"/>
+      <c r="D9" s="204"/>
+      <c r="E9" s="204"/>
       <c r="F9" s="83" t="s">
         <v>115</v>
       </c>
@@ -4503,18 +4507,18 @@
         <v>13</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="182"/>
+      <c r="J9" s="191"/>
     </row>
     <row r="10" spans="1:10" ht="120.75" customHeight="1">
       <c r="A10" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="195"/>
+      <c r="B10" s="204"/>
       <c r="C10" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="195"/>
-      <c r="E10" s="195"/>
+      <c r="D10" s="204"/>
+      <c r="E10" s="204"/>
       <c r="F10" s="83" t="s">
         <v>116</v>
       </c>
@@ -4525,18 +4529,18 @@
         <v>13</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="182"/>
+      <c r="J10" s="191"/>
     </row>
     <row r="11" spans="1:10" ht="119.25" customHeight="1">
       <c r="A11" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="196"/>
+      <c r="B11" s="205"/>
       <c r="C11" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="196"/>
-      <c r="E11" s="196"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="205"/>
       <c r="F11" s="83" t="s">
         <v>117</v>
       </c>
@@ -4547,7 +4551,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="182"/>
+      <c r="J11" s="191"/>
     </row>
     <row r="12" spans="1:10" ht="186.75" customHeight="1" thickBot="1">
       <c r="A12" s="102" t="s">
@@ -4575,7 +4579,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="20"/>
-      <c r="J12" s="182"/>
+      <c r="J12" s="191"/>
     </row>
     <row r="13" spans="1:10" ht="160.5" customHeight="1">
       <c r="A13" s="100" t="s">
@@ -4603,7 +4607,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="63"/>
-      <c r="J13" s="182"/>
+      <c r="J13" s="191"/>
     </row>
     <row r="14" spans="1:10" ht="138" customHeight="1" thickBot="1">
       <c r="A14" s="101" t="s">
@@ -4631,7 +4635,7 @@
         <v>13</v>
       </c>
       <c r="I14" s="61"/>
-      <c r="J14" s="183"/>
+      <c r="J14" s="192"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="98"/>
@@ -4774,7 +4778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -4794,43 +4798,43 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="193" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="186"/>
-      <c r="F2" s="190" t="s">
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="195"/>
+      <c r="F2" s="199" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="191"/>
+      <c r="G2" s="200"/>
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="196" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="188"/>
-      <c r="D3" s="189"/>
-      <c r="F3" s="192" t="s">
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="F3" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="G3" s="193"/>
+      <c r="G3" s="202"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A5" s="177" t="s">
+      <c r="A5" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="178"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
-      <c r="G5" s="178"/>
-      <c r="H5" s="178"/>
-      <c r="I5" s="178"/>
-      <c r="J5" s="179"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="161"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1">
       <c r="A6" s="26" t="s">
@@ -4865,25 +4869,25 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" customHeight="1">
-      <c r="A7" s="174" t="s">
+      <c r="A7" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="201" t="s">
+      <c r="B7" s="214" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="203" t="s">
+      <c r="C7" s="216" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="200" t="s">
+      <c r="E7" s="213" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="198" t="s">
+      <c r="F7" s="211" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="198" t="s">
+      <c r="G7" s="211" t="s">
         <v>96</v>
       </c>
       <c r="H7" s="78" t="s">
@@ -4893,15 +4897,15 @@
       <c r="J7" s="107"/>
     </row>
     <row r="8" spans="1:10" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A8" s="173"/>
-      <c r="B8" s="202"/>
-      <c r="C8" s="202"/>
+      <c r="A8" s="165"/>
+      <c r="B8" s="215"/>
+      <c r="C8" s="215"/>
       <c r="D8" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="175"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="199"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="175"/>
+      <c r="G8" s="212"/>
       <c r="H8" s="79" t="s">
         <v>13</v>
       </c>
@@ -4909,25 +4913,25 @@
       <c r="J8" s="109"/>
     </row>
     <row r="9" spans="1:10" ht="68.25" customHeight="1">
-      <c r="A9" s="172" t="s">
+      <c r="A9" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="154" t="s">
+      <c r="C9" s="156" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="220" t="s">
+      <c r="E9" s="154" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="198" t="s">
+      <c r="F9" s="211" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="198" t="s">
+      <c r="G9" s="211" t="s">
         <v>95</v>
       </c>
       <c r="H9" s="72" t="s">
@@ -4937,60 +4941,60 @@
       <c r="J9" s="109"/>
     </row>
     <row r="10" spans="1:10" ht="69" customHeight="1" thickBot="1">
-      <c r="A10" s="173"/>
-      <c r="B10" s="175"/>
-      <c r="C10" s="175"/>
-      <c r="D10" s="222" t="s">
+      <c r="A10" s="165"/>
+      <c r="B10" s="157"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="175"/>
-      <c r="F10" s="199"/>
-      <c r="G10" s="199"/>
-      <c r="H10" s="222" t="s">
+      <c r="E10" s="157"/>
+      <c r="F10" s="212"/>
+      <c r="G10" s="212"/>
+      <c r="H10" s="122" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="74"/>
       <c r="J10" s="108"/>
     </row>
     <row r="11" spans="1:10" ht="87" customHeight="1">
-      <c r="A11" s="232" t="s">
+      <c r="A11" s="209" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="220" t="s">
+      <c r="B11" s="154" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="230" t="s">
+      <c r="C11" s="207" t="s">
         <v>144</v>
       </c>
       <c r="D11" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="220" t="s">
+      <c r="E11" s="154" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="230" t="s">
+      <c r="F11" s="207" t="s">
         <v>149</v>
       </c>
-      <c r="G11" s="230" t="s">
+      <c r="G11" s="207" t="s">
         <v>150</v>
       </c>
-      <c r="H11" s="218" t="s">
+      <c r="H11" s="121" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="51"/>
       <c r="J11" s="52"/>
     </row>
     <row r="12" spans="1:10" ht="86.25" customHeight="1" thickBot="1">
-      <c r="A12" s="233"/>
-      <c r="B12" s="221"/>
-      <c r="C12" s="234"/>
-      <c r="D12" s="222" t="s">
+      <c r="A12" s="210"/>
+      <c r="B12" s="155"/>
+      <c r="C12" s="208"/>
+      <c r="D12" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="221"/>
-      <c r="F12" s="234"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="222" t="s">
+      <c r="E12" s="155"/>
+      <c r="F12" s="208"/>
+      <c r="G12" s="175"/>
+      <c r="H12" s="122" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="58"/>
@@ -5002,7 +5006,7 @@
       <c r="C13" s="13"/>
       <c r="D13" s="18"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="231"/>
+      <c r="F13" s="130"/>
       <c r="G13" s="18"/>
       <c r="H13" s="2"/>
       <c r="I13" s="80"/>
@@ -5154,11 +5158,8 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
@@ -5175,8 +5176,11 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5207,28 +5211,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="187" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
-      <c r="F2" s="190" t="s">
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="189"/>
+      <c r="F2" s="199" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="191"/>
+      <c r="G2" s="200"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="225" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="205"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="206"/>
-      <c r="F3" s="207" t="s">
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="227"/>
+      <c r="F3" s="228" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="208"/>
+      <c r="G3" s="229"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="117"/>
@@ -5261,18 +5265,18 @@
       <c r="H6" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="18.75">
-      <c r="A8" s="209" t="s">
+      <c r="A8" s="230" t="s">
         <v>131</v>
       </c>
-      <c r="B8" s="209"/>
-      <c r="C8" s="209"/>
-      <c r="D8" s="209"/>
-      <c r="E8" s="209"/>
-      <c r="F8" s="209"/>
-      <c r="G8" s="209"/>
-      <c r="H8" s="209"/>
-      <c r="I8" s="209"/>
-      <c r="J8" s="209"/>
+      <c r="B8" s="230"/>
+      <c r="C8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
+      <c r="G8" s="230"/>
+      <c r="H8" s="230"/>
+      <c r="I8" s="230"/>
+      <c r="J8" s="230"/>
     </row>
     <row r="9" spans="1:10" ht="30">
       <c r="A9" s="113" t="s">
@@ -5316,23 +5320,23 @@
       <c r="C10" s="118" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="210" t="s">
+      <c r="D10" s="217" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="212" t="s">
+      <c r="E10" s="219" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="G10" s="216" t="s">
+      <c r="G10" s="223" t="s">
         <v>138</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="214" t="s">
+      <c r="J10" s="221" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5346,17 +5350,17 @@
       <c r="C11" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="211"/>
-      <c r="E11" s="213"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="220"/>
       <c r="F11" s="118" t="s">
         <v>139</v>
       </c>
-      <c r="G11" s="217"/>
+      <c r="G11" s="224"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="215"/>
+      <c r="J11" s="222"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="119" t="s">

</xml_diff>